<commit_message>
Removed some dupes from vocab, corrected some types in vocab.def, updated documentation to match
</commit_message>
<xml_diff>
--- a/LanguageResources/docs/OpenSextant Entities.xlsx
+++ b/LanguageResources/docs/OpenSextant Entities.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="27660" windowHeight="12150" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="27660" windowHeight="12150"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="1" r:id="rId1"/>
     <sheet name="Hierarchy Roots" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$G$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$J$146</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="209">
   <si>
     <t>Crime</t>
   </si>
@@ -239,9 +239,6 @@
     <t>Object.vehicle.aircraft.helicopter</t>
   </si>
   <si>
-    <t>MiltaryVehicle</t>
-  </si>
-  <si>
     <t>Object</t>
   </si>
   <si>
@@ -413,18 +410,6 @@
     <t>PersonName</t>
   </si>
   <si>
-    <t>PersonNameFragment</t>
-  </si>
-  <si>
-    <t>Person.name.nameFragment</t>
-  </si>
-  <si>
-    <t>PersonNameSuffix</t>
-  </si>
-  <si>
-    <t>Person.name.nameSuffix</t>
-  </si>
-  <si>
     <t>PersonRelation</t>
   </si>
   <si>
@@ -452,18 +437,6 @@
     <t>Person.name.title.religiousTitle</t>
   </si>
   <si>
-    <t>ChemicalElement</t>
-  </si>
-  <si>
-    <t>Substance.chemicalElement</t>
-  </si>
-  <si>
-    <t>ChemicalPart</t>
-  </si>
-  <si>
-    <t>Substance.chemicalPart</t>
-  </si>
-  <si>
     <t>Chemical</t>
   </si>
   <si>
@@ -485,12 +458,6 @@
     <t>Substance</t>
   </si>
   <si>
-    <t>AMPM</t>
-  </si>
-  <si>
-    <t>Time.ampm</t>
-  </si>
-  <si>
     <t>DayOfWeek</t>
   </si>
   <si>
@@ -669,6 +636,15 @@
   </si>
   <si>
     <t>Hierarchy root</t>
+  </si>
+  <si>
+    <t>EmergencyVehicle</t>
+  </si>
+  <si>
+    <t>Object.vehicle.emergencyVehicle</t>
+  </si>
+  <si>
+    <t>Object.vehicle.militaryVehicle.armoredVehicle</t>
   </si>
 </sst>
 </file>
@@ -1007,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,25 +1002,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" t="s">
         <v>204</v>
       </c>
-      <c r="D1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E1" t="s">
-        <v>214</v>
-      </c>
-      <c r="F1" t="s">
-        <v>215</v>
-      </c>
       <c r="G1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1055,10 +1031,10 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G2" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1069,10 +1045,10 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1083,10 +1059,10 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G4" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1097,10 +1073,10 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1111,10 +1087,10 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G6" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1125,10 +1101,10 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G7" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1139,10 +1115,10 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G8" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1153,10 +1129,10 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G9" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1167,10 +1143,10 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G10" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1181,10 +1157,10 @@
         <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G11" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1195,10 +1171,10 @@
         <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1209,10 +1185,10 @@
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G13" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1223,10 +1199,10 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G14" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,10 +1213,10 @@
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G15" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1251,10 +1227,10 @@
         <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G16" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1265,10 +1241,10 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G17" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1279,10 +1255,10 @@
         <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G18" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1293,10 +1269,10 @@
         <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G19" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1307,10 +1283,10 @@
         <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G20" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1321,10 +1297,10 @@
         <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G21" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1335,10 +1311,10 @@
         <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G22" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1349,56 +1325,56 @@
         <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G23" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D24" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E24" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="F24" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G24" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C25" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D25" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E25" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="F25" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G25" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1409,10 +1385,10 @@
         <v>36</v>
       </c>
       <c r="F26" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G26" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1423,10 +1399,10 @@
         <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G27" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1437,10 +1413,10 @@
         <v>38</v>
       </c>
       <c r="F28" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G28" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1451,10 +1427,10 @@
         <v>40</v>
       </c>
       <c r="F29" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G29" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1465,10 +1441,10 @@
         <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G30" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1479,89 +1455,89 @@
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G31" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B32" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F32" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G32" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B33" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="F33" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G33" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B34" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="E34" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="F34" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G34" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35" t="s">
+        <v>188</v>
+      </c>
+      <c r="G35" t="s">
         <v>197</v>
-      </c>
-      <c r="B35" t="s">
-        <v>198</v>
-      </c>
-      <c r="E35" t="s">
-        <v>199</v>
-      </c>
-      <c r="F35" t="s">
-        <v>199</v>
-      </c>
-      <c r="G35" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="E36" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="F36" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G36" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1572,10 +1548,10 @@
         <v>46</v>
       </c>
       <c r="F37" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G37" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1586,80 +1562,80 @@
         <v>48</v>
       </c>
       <c r="F38" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G38" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B39" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="F39" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G39" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B40" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F40" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G40" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B41" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F41" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G41" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B42" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="F42" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G42" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F43" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G43" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1670,10 +1646,10 @@
         <v>54</v>
       </c>
       <c r="F44" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G44" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1684,10 +1660,10 @@
         <v>58</v>
       </c>
       <c r="F45" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G45" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1698,10 +1674,10 @@
         <v>62</v>
       </c>
       <c r="F46" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G46" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1712,10 +1688,10 @@
         <v>64</v>
       </c>
       <c r="F47" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G47" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1726,10 +1702,10 @@
         <v>66</v>
       </c>
       <c r="F48" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G48" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1740,10 +1716,10 @@
         <v>68</v>
       </c>
       <c r="F49" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G49" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1754,69 +1730,69 @@
         <v>60</v>
       </c>
       <c r="F50" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G50" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
         <v>81</v>
       </c>
-      <c r="B51" t="s">
-        <v>82</v>
-      </c>
       <c r="F51" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G51" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B52" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="F52" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G52" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" t="s">
         <v>75</v>
       </c>
-      <c r="B53" t="s">
-        <v>76</v>
-      </c>
       <c r="E53" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="F53" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G53" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" t="s">
         <v>75</v>
       </c>
-      <c r="B54" t="s">
-        <v>76</v>
-      </c>
       <c r="F54" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G54" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1827,24 +1803,24 @@
         <v>70</v>
       </c>
       <c r="F55" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G55" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" t="s">
         <v>83</v>
       </c>
-      <c r="B56" t="s">
-        <v>84</v>
-      </c>
       <c r="F56" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G56" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1855,10 +1831,10 @@
         <v>50</v>
       </c>
       <c r="F57" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G57" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1869,10 +1845,10 @@
         <v>51</v>
       </c>
       <c r="F58" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G58" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -1883,10 +1859,10 @@
         <v>52</v>
       </c>
       <c r="F59" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G59" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -1897,846 +1873,787 @@
         <v>72</v>
       </c>
       <c r="F60" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G60" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>206</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>207</v>
       </c>
       <c r="F61" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G61" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
         <v>56</v>
       </c>
       <c r="F62" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G62" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>78</v>
-      </c>
-      <c r="F63" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="G63" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F64" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G64" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F65" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G65" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B66" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F66" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G66" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F67" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G67" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B68" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F68" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G68" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B69" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F69" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G69" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B70" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F70" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G70" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B71" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F71" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G71" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F72" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G72" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F73" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G73" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B74" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F74" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G74" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B75" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="F75" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G75" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F76" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G76" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>211</v>
+        <v>92</v>
       </c>
       <c r="B77" t="s">
-        <v>212</v>
+        <v>102</v>
       </c>
       <c r="F77" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G77" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>93</v>
+        <v>200</v>
       </c>
       <c r="B78" t="s">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="F78" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G78" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B79" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F79" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G79" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B80" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F80" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G80" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F81" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G81" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="B82" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="F82" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G82" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="F83" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G83" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>113</v>
+      </c>
+      <c r="B84" t="s">
         <v>114</v>
       </c>
-      <c r="B84" t="s">
-        <v>116</v>
-      </c>
       <c r="F84" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G84" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F85" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G85" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B86" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F86" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G86" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B87" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F87" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G87" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B88" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F88" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G88" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B89" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="F89" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G89" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B90" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F90" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G90" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B91" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F91" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G91" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B92" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F92" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G92" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B93" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F93" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G93" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B94" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F94" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G94" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B95" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F95" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G95" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B96" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F96" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G96" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B97" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F97" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G97" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B98" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F98" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G98" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B99" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F99" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G99" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>132</v>
+      </c>
+      <c r="B100" t="s">
         <v>137</v>
       </c>
-      <c r="B100" t="s">
-        <v>141</v>
-      </c>
       <c r="F100" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G100" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B101" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F101" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G101" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B102" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F102" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G102" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B103" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="F103" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G103" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B104" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="F104" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G104" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B105" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F105" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G105" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>143</v>
+      </c>
+      <c r="B106" t="s">
         <v>144</v>
       </c>
-      <c r="B106" t="s">
-        <v>145</v>
-      </c>
       <c r="F106" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G106" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="B107" t="s">
-        <v>147</v>
+        <v>163</v>
+      </c>
+      <c r="C107" t="s">
+        <v>181</v>
+      </c>
+      <c r="E107" t="s">
+        <v>188</v>
       </c>
       <c r="F107" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G107" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B108" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="F108" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G108" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B109" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F109" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G109" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B110" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F110" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G110" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="B111" t="s">
-        <v>174</v>
-      </c>
-      <c r="C111" t="s">
-        <v>192</v>
-      </c>
-      <c r="E111" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F111" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G111" t="s">
-        <v>201</v>
+        <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="B112" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="F112" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G112" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B113" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F113" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G113" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B114" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="F114" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G114" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>206</v>
+        <v>154</v>
       </c>
       <c r="B115" t="s">
-        <v>207</v>
+        <v>155</v>
       </c>
       <c r="F115" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G115" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>161</v>
-      </c>
-      <c r="B116" t="s">
-        <v>162</v>
-      </c>
-      <c r="F116" t="s">
-        <v>199</v>
-      </c>
-      <c r="G116" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>163</v>
-      </c>
-      <c r="B117" t="s">
-        <v>164</v>
-      </c>
-      <c r="F117" t="s">
-        <v>199</v>
-      </c>
-      <c r="G117" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>181</v>
-      </c>
-      <c r="B118" t="s">
-        <v>180</v>
-      </c>
-      <c r="F118" t="s">
-        <v>199</v>
-      </c>
-      <c r="G118" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>165</v>
-      </c>
-      <c r="B119" t="s">
-        <v>166</v>
-      </c>
-      <c r="F119" t="s">
-        <v>199</v>
-      </c>
-      <c r="G119" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G123"/>
+  <autoFilter ref="A1:J146"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2746,7 +2663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -2757,12 +2674,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -2772,7 +2689,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -2787,27 +2704,27 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug that was creating duplicate Entities. Added simple Percentage,Distance,Weight and Area SimpleEntities Added some vocab
</commit_message>
<xml_diff>
--- a/LanguageResources/docs/OpenSextant Entities.xlsx
+++ b/LanguageResources/docs/OpenSextant Entities.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Hierarchy Roots" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$J$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$G$116</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="211">
   <si>
     <t>Crime</t>
   </si>
@@ -452,9 +452,6 @@
     <t>Material</t>
   </si>
   <si>
-    <t>Substance.Material</t>
-  </si>
-  <si>
     <t>Substance</t>
   </si>
   <si>
@@ -479,9 +476,6 @@
     <t>Season</t>
   </si>
   <si>
-    <t>Time.Season</t>
-  </si>
-  <si>
     <t>TimePhrase</t>
   </si>
   <si>
@@ -645,6 +639,18 @@
   </si>
   <si>
     <t>Object.vehicle.militaryVehicle.armoredVehicle</t>
+  </si>
+  <si>
+    <t>Spacecraft</t>
+  </si>
+  <si>
+    <t>Object.vehicle.spacecraft</t>
+  </si>
+  <si>
+    <t>Substance.material</t>
+  </si>
+  <si>
+    <t>Time.season</t>
   </si>
 </sst>
 </file>
@@ -983,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,25 +1008,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" t="s">
         <v>156</v>
-      </c>
-      <c r="B1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1031,10 +1037,10 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1045,10 +1051,10 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1059,10 +1065,10 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1073,10 +1079,10 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1087,10 +1093,10 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1101,10 +1107,10 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1115,10 +1121,10 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1129,10 +1135,10 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1143,10 +1149,10 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1157,10 +1163,10 @@
         <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1171,10 +1177,10 @@
         <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1185,10 +1191,10 @@
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1199,10 +1205,10 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1213,10 +1219,10 @@
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1227,10 +1233,10 @@
         <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1241,10 +1247,10 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1255,10 +1261,10 @@
         <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1269,10 +1275,10 @@
         <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1283,10 +1289,10 @@
         <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1297,10 +1303,10 @@
         <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1311,10 +1317,10 @@
         <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1325,56 +1331,56 @@
         <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1385,10 +1391,10 @@
         <v>36</v>
       </c>
       <c r="F26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1399,10 +1405,10 @@
         <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1413,10 +1419,10 @@
         <v>38</v>
       </c>
       <c r="F28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1427,10 +1433,10 @@
         <v>40</v>
       </c>
       <c r="F29" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1441,10 +1447,10 @@
         <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1455,89 +1461,89 @@
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F32" t="s">
+        <v>186</v>
+      </c>
+      <c r="G32" t="s">
         <v>166</v>
-      </c>
-      <c r="F32" t="s">
-        <v>188</v>
-      </c>
-      <c r="G32" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B33" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G33" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B34" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E34" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F34" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G34" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E35" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F35" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G35" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E36" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F36" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1548,10 +1554,10 @@
         <v>46</v>
       </c>
       <c r="F37" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1562,66 +1568,66 @@
         <v>48</v>
       </c>
       <c r="F38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G39" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B40" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F40" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G40" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B41" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F41" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G41" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F42" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G42" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,10 +1638,10 @@
         <v>73</v>
       </c>
       <c r="F43" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1646,10 +1652,10 @@
         <v>54</v>
       </c>
       <c r="F44" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1660,10 +1666,10 @@
         <v>58</v>
       </c>
       <c r="F45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1674,10 +1680,10 @@
         <v>62</v>
       </c>
       <c r="F46" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G46" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1688,10 +1694,10 @@
         <v>64</v>
       </c>
       <c r="F47" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1702,10 +1708,10 @@
         <v>66</v>
       </c>
       <c r="F48" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G48" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1716,10 +1722,10 @@
         <v>68</v>
       </c>
       <c r="F49" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G49" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1730,10 +1736,10 @@
         <v>60</v>
       </c>
       <c r="F50" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G50" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1744,24 +1750,24 @@
         <v>81</v>
       </c>
       <c r="F51" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B52" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F52" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G52" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1772,13 +1778,13 @@
         <v>75</v>
       </c>
       <c r="E53" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F53" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G53" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1789,10 +1795,10 @@
         <v>75</v>
       </c>
       <c r="F54" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1803,10 +1809,10 @@
         <v>70</v>
       </c>
       <c r="F55" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G55" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1817,10 +1823,10 @@
         <v>83</v>
       </c>
       <c r="F56" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G56" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1831,10 +1837,10 @@
         <v>50</v>
       </c>
       <c r="F57" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G57" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1845,10 +1851,10 @@
         <v>51</v>
       </c>
       <c r="F58" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G58" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -1859,10 +1865,10 @@
         <v>52</v>
       </c>
       <c r="F59" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G59" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -1873,24 +1879,24 @@
         <v>72</v>
       </c>
       <c r="F60" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G60" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B61" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F61" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G61" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -1901,10 +1907,10 @@
         <v>56</v>
       </c>
       <c r="F62" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G62" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -1912,10 +1918,13 @@
         <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>208</v>
+        <v>206</v>
+      </c>
+      <c r="F63" t="s">
+        <v>186</v>
       </c>
       <c r="G63" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -1926,164 +1935,164 @@
         <v>77</v>
       </c>
       <c r="F64" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G64" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>207</v>
       </c>
       <c r="B65" t="s">
-        <v>79</v>
+        <v>208</v>
       </c>
       <c r="F65" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G65" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="F66" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G66" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F67" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G67" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F68" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G68" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F69" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G69" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B70" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F70" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G70" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F71" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G71" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B72" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F72" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G72" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F73" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G73" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B74" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="F74" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G74" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F75" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G75" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2091,13 +2100,13 @@
         <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="F76" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G76" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2105,41 +2114,41 @@
         <v>92</v>
       </c>
       <c r="B77" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F77" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G77" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>200</v>
+        <v>92</v>
       </c>
       <c r="B78" t="s">
-        <v>201</v>
+        <v>102</v>
       </c>
       <c r="F78" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G78" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>198</v>
       </c>
       <c r="B79" t="s">
-        <v>103</v>
+        <v>199</v>
       </c>
       <c r="F79" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G79" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2147,69 +2156,69 @@
         <v>92</v>
       </c>
       <c r="B80" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F80" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G80" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B81" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="F81" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G81" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B82" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F82" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G82" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="F83" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G83" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B84" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="F84" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G84" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2217,13 +2226,13 @@
         <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F85" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G85" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2231,153 +2240,153 @@
         <v>113</v>
       </c>
       <c r="B86" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F86" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G86" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B87" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="F87" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G87" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F88" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G88" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F89" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G89" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B90" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="F90" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G90" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B91" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="F91" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G91" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B92" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F92" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G92" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B93" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F93" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G93" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F94" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G94" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B95" t="s">
         <v>128</v>
       </c>
       <c r="F95" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G95" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B96" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F96" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G96" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -2385,13 +2394,13 @@
         <v>132</v>
       </c>
       <c r="B97" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F97" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G97" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -2399,13 +2408,13 @@
         <v>132</v>
       </c>
       <c r="B98" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F98" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G98" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -2413,13 +2422,13 @@
         <v>132</v>
       </c>
       <c r="B99" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F99" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G99" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -2427,13 +2436,13 @@
         <v>132</v>
       </c>
       <c r="B100" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F100" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G100" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -2441,219 +2450,233 @@
         <v>132</v>
       </c>
       <c r="B101" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F101" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G101" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B102" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="F102" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G102" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B103" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F103" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G103" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B104" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F104" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G104" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B105" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F105" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G105" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B106" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F106" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G106" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B107" t="s">
-        <v>163</v>
-      </c>
-      <c r="C107" t="s">
-        <v>181</v>
-      </c>
-      <c r="E107" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="F107" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G107" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B108" t="s">
-        <v>163</v>
+        <v>161</v>
+      </c>
+      <c r="C108" t="s">
+        <v>179</v>
+      </c>
+      <c r="E108" t="s">
+        <v>186</v>
       </c>
       <c r="F108" t="s">
+        <v>186</v>
+      </c>
+      <c r="G108" t="s">
         <v>188</v>
-      </c>
-      <c r="G108" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B109" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="F109" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G109" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B110" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F110" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G110" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
       <c r="B111" t="s">
-        <v>196</v>
+        <v>148</v>
       </c>
       <c r="F111" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G111" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="B112" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="F112" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G112" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B113" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F113" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G113" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="B114" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="F114" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G114" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B115" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="F115" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G115" t="s">
-        <v>159</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>152</v>
+      </c>
+      <c r="B116" t="s">
+        <v>153</v>
+      </c>
+      <c r="F116" t="s">
+        <v>186</v>
+      </c>
+      <c r="G116" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J146"/>
+  <autoFilter ref="A1:G116"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2674,12 +2697,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -2689,7 +2712,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -2719,12 +2742,12 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated docs to included new Simple Entities
</commit_message>
<xml_diff>
--- a/LanguageResources/docs/OpenSextant Entities.xlsx
+++ b/LanguageResources/docs/OpenSextant Entities.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Hierarchy Roots" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$G$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$G$118</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="216">
   <si>
     <t>Crime</t>
   </si>
@@ -596,9 +596,6 @@
     <t>Type specific features [ featurename(object type)]</t>
   </si>
   <si>
-    <t>Information.identifier.abbreviation</t>
-  </si>
-  <si>
     <t>TimePeriod</t>
   </si>
   <si>
@@ -651,6 +648,24 @@
   </si>
   <si>
     <t>Time.season</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Geo.distance</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Geo.area</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Attribute.weight</t>
   </si>
 </sst>
 </file>
@@ -989,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,10 +1035,10 @@
         <v>163</v>
       </c>
       <c r="E1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" t="s">
         <v>201</v>
-      </c>
-      <c r="F1" t="s">
-        <v>202</v>
       </c>
       <c r="G1" t="s">
         <v>156</v>
@@ -1185,52 +1200,52 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>214</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>215</v>
       </c>
       <c r="F13" t="s">
         <v>186</v>
       </c>
       <c r="G13" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>212</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>213</v>
       </c>
       <c r="F14" t="s">
         <v>186</v>
       </c>
       <c r="G14" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>210</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>211</v>
       </c>
       <c r="F15" t="s">
         <v>186</v>
       </c>
       <c r="G15" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
         <v>186</v>
@@ -1244,7 +1259,7 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
         <v>186</v>
@@ -1258,7 +1273,7 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
         <v>186</v>
@@ -1272,7 +1287,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
         <v>186</v>
@@ -1286,7 +1301,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F20" t="s">
         <v>186</v>
@@ -1300,7 +1315,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F21" t="s">
         <v>186</v>
@@ -1314,7 +1329,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F22" t="s">
         <v>186</v>
@@ -1328,7 +1343,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
         <v>186</v>
@@ -1339,56 +1354,38 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>158</v>
-      </c>
-      <c r="C24" t="s">
-        <v>180</v>
-      </c>
-      <c r="D24" t="s">
-        <v>186</v>
-      </c>
-      <c r="E24" t="s">
-        <v>186</v>
+        <v>32</v>
       </c>
       <c r="F24" t="s">
         <v>186</v>
       </c>
       <c r="G24" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>200</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
-      </c>
-      <c r="C25" t="s">
-        <v>181</v>
-      </c>
-      <c r="D25" t="s">
-        <v>186</v>
-      </c>
-      <c r="E25" t="s">
-        <v>186</v>
+        <v>33</v>
       </c>
       <c r="F25" t="s">
         <v>186</v>
       </c>
       <c r="G25" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F26" t="s">
         <v>186</v>
@@ -1399,38 +1396,56 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>159</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>158</v>
+      </c>
+      <c r="C27" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E27" t="s">
+        <v>186</v>
       </c>
       <c r="F27" t="s">
         <v>186</v>
       </c>
       <c r="G27" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>199</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>162</v>
+      </c>
+      <c r="C28" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" t="s">
+        <v>186</v>
+      </c>
+      <c r="E28" t="s">
+        <v>186</v>
       </c>
       <c r="F28" t="s">
         <v>186</v>
       </c>
       <c r="G28" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F29" t="s">
         <v>186</v>
@@ -1441,10 +1456,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F30" t="s">
         <v>186</v>
@@ -1455,10 +1470,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F31" t="s">
         <v>186</v>
@@ -1469,72 +1484,66 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>164</v>
+        <v>40</v>
       </c>
       <c r="F32" t="s">
         <v>186</v>
       </c>
       <c r="G32" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>192</v>
+        <v>41</v>
       </c>
       <c r="F33" t="s">
         <v>186</v>
       </c>
       <c r="G33" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
-      </c>
-      <c r="E34" t="s">
-        <v>186</v>
+        <v>44</v>
       </c>
       <c r="F34" t="s">
         <v>186</v>
       </c>
       <c r="G34" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="B35" t="s">
-        <v>185</v>
-      </c>
-      <c r="E35" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="F35" t="s">
         <v>186</v>
       </c>
       <c r="G35" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B36" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E36" t="s">
         <v>186</v>
@@ -1543,71 +1552,77 @@
         <v>186</v>
       </c>
       <c r="G36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>185</v>
+      </c>
+      <c r="E37" t="s">
+        <v>186</v>
       </c>
       <c r="F37" t="s">
         <v>186</v>
       </c>
       <c r="G37" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>183</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>182</v>
+      </c>
+      <c r="E38" t="s">
+        <v>186</v>
       </c>
       <c r="F38" t="s">
         <v>186</v>
       </c>
       <c r="G38" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>169</v>
+        <v>46</v>
       </c>
       <c r="F39" t="s">
         <v>186</v>
       </c>
       <c r="G39" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>175</v>
+        <v>48</v>
       </c>
       <c r="F40" t="s">
         <v>186</v>
       </c>
       <c r="G40" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B41" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F41" t="s">
         <v>186</v>
@@ -1618,10 +1633,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F42" t="s">
         <v>186</v>
@@ -1632,38 +1647,38 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>172</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="F43" t="s">
         <v>186</v>
       </c>
       <c r="G43" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="F44" t="s">
         <v>186</v>
       </c>
       <c r="G44" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="F45" t="s">
         <v>186</v>
@@ -1674,10 +1689,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F46" t="s">
         <v>186</v>
@@ -1688,10 +1703,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F47" t="s">
         <v>186</v>
@@ -1702,10 +1717,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F48" t="s">
         <v>186</v>
@@ -1716,10 +1731,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F49" t="s">
         <v>186</v>
@@ -1730,10 +1745,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F50" t="s">
         <v>186</v>
@@ -1744,10 +1759,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="F51" t="s">
         <v>186</v>
@@ -1758,10 +1773,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>197</v>
+        <v>60</v>
       </c>
       <c r="F52" t="s">
         <v>186</v>
@@ -1772,69 +1787,69 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B53" t="s">
-        <v>75</v>
-      </c>
-      <c r="E53" t="s">
-        <v>186</v>
+        <v>81</v>
       </c>
       <c r="F53" t="s">
         <v>186</v>
       </c>
       <c r="G53" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>195</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>196</v>
       </c>
       <c r="F54" t="s">
         <v>186</v>
       </c>
       <c r="G54" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>75</v>
+      </c>
+      <c r="E55" t="s">
+        <v>186</v>
       </c>
       <c r="F55" t="s">
         <v>186</v>
       </c>
       <c r="G55" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F56" t="s">
         <v>186</v>
       </c>
       <c r="G56" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F57" t="s">
         <v>186</v>
@@ -1845,10 +1860,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B58" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="F58" t="s">
         <v>186</v>
@@ -1862,7 +1877,7 @@
         <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F59" t="s">
         <v>186</v>
@@ -1873,10 +1888,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="F60" t="s">
         <v>186</v>
@@ -1887,10 +1902,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>204</v>
+        <v>49</v>
       </c>
       <c r="B61" t="s">
-        <v>205</v>
+        <v>52</v>
       </c>
       <c r="F61" t="s">
         <v>186</v>
@@ -1901,10 +1916,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="F62" t="s">
         <v>186</v>
@@ -1915,10 +1930,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>55</v>
+        <v>203</v>
       </c>
       <c r="B63" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F63" t="s">
         <v>186</v>
@@ -1929,10 +1944,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="F64" t="s">
         <v>186</v>
@@ -1943,10 +1958,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>207</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F65" t="s">
         <v>186</v>
@@ -1957,10 +1972,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F66" t="s">
         <v>186</v>
@@ -1971,10 +1986,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>206</v>
       </c>
       <c r="B67" t="s">
-        <v>91</v>
+        <v>207</v>
       </c>
       <c r="F67" t="s">
         <v>186</v>
@@ -1985,10 +2000,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F68" t="s">
         <v>186</v>
@@ -1999,10 +2014,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B69" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F69" t="s">
         <v>186</v>
@@ -2013,10 +2028,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F70" t="s">
         <v>186</v>
@@ -2027,10 +2042,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F71" t="s">
         <v>186</v>
@@ -2041,10 +2056,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F72" t="s">
         <v>186</v>
@@ -2055,10 +2070,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B73" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F73" t="s">
         <v>186</v>
@@ -2069,10 +2084,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F74" t="s">
         <v>186</v>
@@ -2083,10 +2098,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B75" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F75" t="s">
         <v>186</v>
@@ -2100,7 +2115,7 @@
         <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="F76" t="s">
         <v>186</v>
@@ -2111,10 +2126,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="F77" t="s">
         <v>186</v>
@@ -2128,7 +2143,7 @@
         <v>92</v>
       </c>
       <c r="B78" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="F78" t="s">
         <v>186</v>
@@ -2139,10 +2154,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>198</v>
+        <v>92</v>
       </c>
       <c r="B79" t="s">
-        <v>199</v>
+        <v>95</v>
       </c>
       <c r="F79" t="s">
         <v>186</v>
@@ -2156,7 +2171,7 @@
         <v>92</v>
       </c>
       <c r="B80" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F80" t="s">
         <v>186</v>
@@ -2167,10 +2182,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="B81" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
       <c r="F81" t="s">
         <v>186</v>
@@ -2181,10 +2196,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F82" t="s">
         <v>186</v>
@@ -2195,10 +2210,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B83" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F83" t="s">
         <v>186</v>
@@ -2209,10 +2224,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="B84" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="F84" t="s">
         <v>186</v>
@@ -2223,10 +2238,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B85" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="F85" t="s">
         <v>186</v>
@@ -2237,10 +2252,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B86" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="F86" t="s">
         <v>186</v>
@@ -2254,7 +2269,7 @@
         <v>113</v>
       </c>
       <c r="B87" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F87" t="s">
         <v>186</v>
@@ -2265,10 +2280,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B88" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F88" t="s">
         <v>186</v>
@@ -2279,10 +2294,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B89" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F89" t="s">
         <v>186</v>
@@ -2293,10 +2308,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B90" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F90" t="s">
         <v>186</v>
@@ -2307,10 +2322,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B91" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F91" t="s">
         <v>186</v>
@@ -2321,10 +2336,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B92" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F92" t="s">
         <v>186</v>
@@ -2335,10 +2350,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B93" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="F93" t="s">
         <v>186</v>
@@ -2349,10 +2364,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F94" t="s">
         <v>186</v>
@@ -2363,10 +2378,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B95" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F95" t="s">
         <v>186</v>
@@ -2377,10 +2392,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B96" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F96" t="s">
         <v>186</v>
@@ -2391,10 +2406,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B97" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F97" t="s">
         <v>186</v>
@@ -2405,10 +2420,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B98" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F98" t="s">
         <v>186</v>
@@ -2422,7 +2437,7 @@
         <v>132</v>
       </c>
       <c r="B99" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F99" t="s">
         <v>186</v>
@@ -2436,7 +2451,7 @@
         <v>132</v>
       </c>
       <c r="B100" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F100" t="s">
         <v>186</v>
@@ -2450,7 +2465,7 @@
         <v>132</v>
       </c>
       <c r="B101" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F101" t="s">
         <v>186</v>
@@ -2464,7 +2479,7 @@
         <v>132</v>
       </c>
       <c r="B102" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F102" t="s">
         <v>186</v>
@@ -2475,10 +2490,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B103" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F103" t="s">
         <v>186</v>
@@ -2489,10 +2504,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B104" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F104" t="s">
         <v>186</v>
@@ -2503,10 +2518,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B105" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F105" t="s">
         <v>186</v>
@@ -2517,10 +2532,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B106" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F106" t="s">
         <v>186</v>
@@ -2531,10 +2546,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B107" t="s">
-        <v>209</v>
+        <v>140</v>
       </c>
       <c r="F107" t="s">
         <v>186</v>
@@ -2545,86 +2560,86 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="B108" t="s">
-        <v>161</v>
-      </c>
-      <c r="C108" t="s">
-        <v>179</v>
-      </c>
-      <c r="E108" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="F108" t="s">
         <v>186</v>
       </c>
       <c r="G108" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B109" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
       <c r="F109" t="s">
         <v>186</v>
       </c>
       <c r="G109" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="B110" t="s">
-        <v>146</v>
+        <v>161</v>
+      </c>
+      <c r="C110" t="s">
+        <v>179</v>
+      </c>
+      <c r="E110" t="s">
+        <v>186</v>
       </c>
       <c r="F110" t="s">
         <v>186</v>
       </c>
       <c r="G110" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B111" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="F111" t="s">
         <v>186</v>
       </c>
       <c r="G111" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>193</v>
+        <v>145</v>
       </c>
       <c r="B112" t="s">
-        <v>194</v>
+        <v>146</v>
       </c>
       <c r="F112" t="s">
         <v>186</v>
       </c>
       <c r="G112" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B113" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F113" t="s">
         <v>186</v>
@@ -2635,48 +2650,80 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="B114" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="F114" t="s">
         <v>186</v>
       </c>
       <c r="G114" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="B115" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="F115" t="s">
         <v>186</v>
       </c>
       <c r="G115" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>151</v>
+      </c>
+      <c r="B116" t="s">
+        <v>209</v>
+      </c>
+      <c r="F116" t="s">
+        <v>186</v>
+      </c>
+      <c r="G116" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>168</v>
+      </c>
+      <c r="B117" t="s">
+        <v>167</v>
+      </c>
+      <c r="F117" t="s">
+        <v>186</v>
+      </c>
+      <c r="G117" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>152</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B118" t="s">
         <v>153</v>
       </c>
-      <c r="F116" t="s">
-        <v>186</v>
-      </c>
-      <c r="G116" t="s">
+      <c r="F118" t="s">
+        <v>186</v>
+      </c>
+      <c r="G118" t="s">
         <v>157</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G116"/>
+  <autoFilter ref="A1:G118">
+    <sortState ref="A2:G118">
+      <sortCondition ref="B1:B118"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2697,7 +2744,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added new OpenSextant_Basic.gapp, updated docs and spreadsheet to match
</commit_message>
<xml_diff>
--- a/LanguageResources/docs/OpenSextant Entities.xlsx
+++ b/LanguageResources/docs/OpenSextant Entities.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Hierarchy Roots" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$G$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$I$118</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="218">
   <si>
     <t>Crime</t>
   </si>
@@ -666,6 +666,12 @@
   </si>
   <si>
     <t>Attribute.weight</t>
+  </si>
+  <si>
+    <t>Geocoords Only</t>
+  </si>
+  <si>
+    <t>Basic</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G118"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,13 +1021,15 @@
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>154</v>
       </c>
@@ -1032,369 +1040,375 @@
         <v>191</v>
       </c>
       <c r="D1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F1" t="s">
         <v>163</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>200</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>201</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>186</v>
-      </c>
-      <c r="G2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>186</v>
-      </c>
-      <c r="G3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>186</v>
+      </c>
+      <c r="I4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>186</v>
+      </c>
+      <c r="I5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" t="s">
-        <v>186</v>
-      </c>
-      <c r="G6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>186</v>
+      </c>
+      <c r="I6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
-        <v>186</v>
-      </c>
-      <c r="G7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>186</v>
+      </c>
+      <c r="I7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
-        <v>186</v>
-      </c>
-      <c r="G8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="F9" t="s">
-        <v>186</v>
-      </c>
-      <c r="G9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>186</v>
+      </c>
+      <c r="I9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
-        <v>186</v>
-      </c>
-      <c r="G10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>186</v>
+      </c>
+      <c r="I10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="F11" t="s">
-        <v>186</v>
-      </c>
-      <c r="G11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>186</v>
+      </c>
+      <c r="I11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="F12" t="s">
-        <v>186</v>
-      </c>
-      <c r="G12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>186</v>
+      </c>
+      <c r="I12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>214</v>
       </c>
       <c r="B13" t="s">
         <v>215</v>
       </c>
-      <c r="F13" t="s">
-        <v>186</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
+        <v>186</v>
+      </c>
+      <c r="I13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>212</v>
       </c>
       <c r="B14" t="s">
         <v>213</v>
       </c>
-      <c r="F14" t="s">
-        <v>186</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I14" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>210</v>
       </c>
       <c r="B15" t="s">
         <v>211</v>
       </c>
-      <c r="F15" t="s">
-        <v>186</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
+        <v>186</v>
+      </c>
+      <c r="I15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
-        <v>186</v>
-      </c>
-      <c r="G16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>186</v>
+      </c>
+      <c r="I16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="F17" t="s">
-        <v>186</v>
-      </c>
-      <c r="G17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>186</v>
+      </c>
+      <c r="I17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="F18" t="s">
-        <v>186</v>
-      </c>
-      <c r="G18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>186</v>
+      </c>
+      <c r="I18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="F19" t="s">
-        <v>186</v>
-      </c>
-      <c r="G19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>186</v>
+      </c>
+      <c r="I19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="F20" t="s">
-        <v>186</v>
-      </c>
-      <c r="G20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>186</v>
+      </c>
+      <c r="I20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="F21" t="s">
-        <v>186</v>
-      </c>
-      <c r="G21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>186</v>
+      </c>
+      <c r="I21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="F22" t="s">
-        <v>186</v>
-      </c>
-      <c r="G22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>186</v>
+      </c>
+      <c r="I22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="F23" t="s">
-        <v>186</v>
-      </c>
-      <c r="G23" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>186</v>
+      </c>
+      <c r="I23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="F24" t="s">
-        <v>186</v>
-      </c>
-      <c r="G24" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>186</v>
+      </c>
+      <c r="I24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
-      <c r="F25" t="s">
-        <v>186</v>
-      </c>
-      <c r="G25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>186</v>
+      </c>
+      <c r="I25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="F26" t="s">
-        <v>186</v>
-      </c>
-      <c r="G26" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>186</v>
+      </c>
+      <c r="I26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>159</v>
       </c>
@@ -1414,10 +1428,16 @@
         <v>186</v>
       </c>
       <c r="G27" t="s">
+        <v>186</v>
+      </c>
+      <c r="H27" t="s">
+        <v>186</v>
+      </c>
+      <c r="I27" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>199</v>
       </c>
@@ -1427,118 +1447,118 @@
       <c r="C28" t="s">
         <v>181</v>
       </c>
-      <c r="D28" t="s">
-        <v>186</v>
-      </c>
-      <c r="E28" t="s">
-        <v>186</v>
-      </c>
       <c r="F28" t="s">
         <v>186</v>
       </c>
       <c r="G28" t="s">
+        <v>186</v>
+      </c>
+      <c r="H28" t="s">
+        <v>186</v>
+      </c>
+      <c r="I28" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="F29" t="s">
-        <v>186</v>
-      </c>
-      <c r="G29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>186</v>
+      </c>
+      <c r="I29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
       <c r="B30" t="s">
         <v>43</v>
       </c>
-      <c r="F30" t="s">
-        <v>186</v>
-      </c>
-      <c r="G30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>186</v>
+      </c>
+      <c r="I30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
       <c r="B31" t="s">
         <v>38</v>
       </c>
-      <c r="F31" t="s">
-        <v>186</v>
-      </c>
-      <c r="G31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>186</v>
+      </c>
+      <c r="I31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
       </c>
-      <c r="F32" t="s">
-        <v>186</v>
-      </c>
-      <c r="G32" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>186</v>
+      </c>
+      <c r="I32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>41</v>
       </c>
-      <c r="F33" t="s">
-        <v>186</v>
-      </c>
-      <c r="G33" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>186</v>
+      </c>
+      <c r="I33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
       <c r="B34" t="s">
         <v>44</v>
       </c>
-      <c r="F34" t="s">
-        <v>186</v>
-      </c>
-      <c r="G34" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>186</v>
+      </c>
+      <c r="I34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>165</v>
       </c>
       <c r="B35" t="s">
         <v>164</v>
       </c>
-      <c r="F35" t="s">
-        <v>186</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
+        <v>186</v>
+      </c>
+      <c r="I35" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>189</v>
       </c>
@@ -1548,14 +1568,17 @@
       <c r="E36" t="s">
         <v>186</v>
       </c>
-      <c r="F36" t="s">
-        <v>186</v>
-      </c>
       <c r="G36" t="s">
+        <v>186</v>
+      </c>
+      <c r="H36" t="s">
+        <v>186</v>
+      </c>
+      <c r="I36" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>184</v>
       </c>
@@ -1565,14 +1588,17 @@
       <c r="E37" t="s">
         <v>186</v>
       </c>
-      <c r="F37" t="s">
-        <v>186</v>
-      </c>
       <c r="G37" t="s">
+        <v>186</v>
+      </c>
+      <c r="H37" t="s">
+        <v>186</v>
+      </c>
+      <c r="I37" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -1582,238 +1608,241 @@
       <c r="E38" t="s">
         <v>186</v>
       </c>
-      <c r="F38" t="s">
-        <v>186</v>
-      </c>
       <c r="G38" t="s">
+        <v>186</v>
+      </c>
+      <c r="H38" t="s">
+        <v>186</v>
+      </c>
+      <c r="I38" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
       <c r="B39" t="s">
         <v>46</v>
       </c>
-      <c r="F39" t="s">
-        <v>186</v>
-      </c>
-      <c r="G39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>186</v>
+      </c>
+      <c r="I39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
       </c>
-      <c r="F40" t="s">
-        <v>186</v>
-      </c>
-      <c r="G40" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>186</v>
+      </c>
+      <c r="I40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>170</v>
       </c>
       <c r="B41" t="s">
         <v>169</v>
       </c>
-      <c r="F41" t="s">
-        <v>186</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
+        <v>186</v>
+      </c>
+      <c r="I41" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>176</v>
       </c>
       <c r="B42" t="s">
         <v>175</v>
       </c>
-      <c r="F42" t="s">
-        <v>186</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
+        <v>186</v>
+      </c>
+      <c r="I42" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>172</v>
       </c>
       <c r="B43" t="s">
         <v>171</v>
       </c>
-      <c r="F43" t="s">
-        <v>186</v>
-      </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
+        <v>186</v>
+      </c>
+      <c r="I43" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>174</v>
       </c>
       <c r="B44" t="s">
         <v>173</v>
       </c>
-      <c r="F44" t="s">
-        <v>186</v>
-      </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
+        <v>186</v>
+      </c>
+      <c r="I44" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>73</v>
       </c>
       <c r="B45" t="s">
         <v>73</v>
       </c>
-      <c r="F45" t="s">
-        <v>186</v>
-      </c>
-      <c r="G45" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>186</v>
+      </c>
+      <c r="I45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
       <c r="B46" t="s">
         <v>54</v>
       </c>
-      <c r="F46" t="s">
-        <v>186</v>
-      </c>
-      <c r="G46" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>186</v>
+      </c>
+      <c r="I46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>57</v>
       </c>
       <c r="B47" t="s">
         <v>58</v>
       </c>
-      <c r="F47" t="s">
-        <v>186</v>
-      </c>
-      <c r="G47" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>186</v>
+      </c>
+      <c r="I47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>61</v>
       </c>
       <c r="B48" t="s">
         <v>62</v>
       </c>
-      <c r="F48" t="s">
-        <v>186</v>
-      </c>
-      <c r="G48" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>186</v>
+      </c>
+      <c r="I48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
       <c r="B49" t="s">
         <v>64</v>
       </c>
-      <c r="F49" t="s">
-        <v>186</v>
-      </c>
-      <c r="G49" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>186</v>
+      </c>
+      <c r="I49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>65</v>
       </c>
       <c r="B50" t="s">
         <v>66</v>
       </c>
-      <c r="F50" t="s">
-        <v>186</v>
-      </c>
-      <c r="G50" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>186</v>
+      </c>
+      <c r="I50" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>67</v>
       </c>
       <c r="B51" t="s">
         <v>68</v>
       </c>
-      <c r="F51" t="s">
-        <v>186</v>
-      </c>
-      <c r="G51" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>186</v>
+      </c>
+      <c r="I51" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
       </c>
-      <c r="F52" t="s">
-        <v>186</v>
-      </c>
-      <c r="G52" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>186</v>
+      </c>
+      <c r="I52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>80</v>
       </c>
       <c r="B53" t="s">
         <v>81</v>
       </c>
-      <c r="F53" t="s">
-        <v>186</v>
-      </c>
-      <c r="G53" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>186</v>
+      </c>
+      <c r="I53" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>195</v>
       </c>
       <c r="B54" t="s">
         <v>196</v>
       </c>
-      <c r="F54" t="s">
-        <v>186</v>
-      </c>
-      <c r="G54" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>186</v>
+      </c>
+      <c r="I54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -1823,770 +1852,773 @@
       <c r="E55" t="s">
         <v>186</v>
       </c>
-      <c r="F55" t="s">
-        <v>186</v>
-      </c>
       <c r="G55" t="s">
+        <v>186</v>
+      </c>
+      <c r="H55" t="s">
+        <v>186</v>
+      </c>
+      <c r="I55" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>74</v>
       </c>
       <c r="B56" t="s">
         <v>75</v>
       </c>
-      <c r="F56" t="s">
-        <v>186</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
+        <v>186</v>
+      </c>
+      <c r="I56" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>69</v>
       </c>
       <c r="B57" t="s">
         <v>70</v>
       </c>
-      <c r="F57" t="s">
-        <v>186</v>
-      </c>
-      <c r="G57" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>186</v>
+      </c>
+      <c r="I57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>82</v>
       </c>
       <c r="B58" t="s">
         <v>83</v>
       </c>
-      <c r="F58" t="s">
-        <v>186</v>
-      </c>
-      <c r="G58" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>186</v>
+      </c>
+      <c r="I58" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>49</v>
       </c>
       <c r="B59" t="s">
         <v>50</v>
       </c>
-      <c r="F59" t="s">
-        <v>186</v>
-      </c>
-      <c r="G59" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>186</v>
+      </c>
+      <c r="I59" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>49</v>
       </c>
       <c r="B60" t="s">
         <v>51</v>
       </c>
-      <c r="F60" t="s">
-        <v>186</v>
-      </c>
-      <c r="G60" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>186</v>
+      </c>
+      <c r="I60" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>49</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
       </c>
-      <c r="F61" t="s">
-        <v>186</v>
-      </c>
-      <c r="G61" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
+        <v>186</v>
+      </c>
+      <c r="I61" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>71</v>
       </c>
       <c r="B62" t="s">
         <v>72</v>
       </c>
-      <c r="F62" t="s">
-        <v>186</v>
-      </c>
-      <c r="G62" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>186</v>
+      </c>
+      <c r="I62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>203</v>
       </c>
       <c r="B63" t="s">
         <v>204</v>
       </c>
-      <c r="F63" t="s">
-        <v>186</v>
-      </c>
-      <c r="G63" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>186</v>
+      </c>
+      <c r="I63" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
       </c>
       <c r="B64" t="s">
         <v>56</v>
       </c>
-      <c r="F64" t="s">
-        <v>186</v>
-      </c>
-      <c r="G64" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" t="s">
+        <v>186</v>
+      </c>
+      <c r="I64" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
       <c r="B65" t="s">
         <v>205</v>
       </c>
-      <c r="F65" t="s">
-        <v>186</v>
-      </c>
-      <c r="G65" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
+        <v>186</v>
+      </c>
+      <c r="I65" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>76</v>
       </c>
       <c r="B66" t="s">
         <v>77</v>
       </c>
-      <c r="F66" t="s">
-        <v>186</v>
-      </c>
-      <c r="G66" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>186</v>
+      </c>
+      <c r="I66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>206</v>
       </c>
       <c r="B67" t="s">
         <v>207</v>
       </c>
-      <c r="F67" t="s">
-        <v>186</v>
-      </c>
-      <c r="G67" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
+        <v>186</v>
+      </c>
+      <c r="I67" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>78</v>
       </c>
       <c r="B68" t="s">
         <v>79</v>
       </c>
-      <c r="F68" t="s">
-        <v>186</v>
-      </c>
-      <c r="G68" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>186</v>
+      </c>
+      <c r="I68" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>90</v>
       </c>
       <c r="B69" t="s">
         <v>91</v>
       </c>
-      <c r="F69" t="s">
-        <v>186</v>
-      </c>
-      <c r="G69" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" t="s">
+        <v>186</v>
+      </c>
+      <c r="I69" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>84</v>
       </c>
       <c r="B70" t="s">
         <v>85</v>
       </c>
-      <c r="F70" t="s">
-        <v>186</v>
-      </c>
-      <c r="G70" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>186</v>
+      </c>
+      <c r="I70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>86</v>
       </c>
       <c r="B71" t="s">
         <v>87</v>
       </c>
-      <c r="F71" t="s">
-        <v>186</v>
-      </c>
-      <c r="G71" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
+        <v>186</v>
+      </c>
+      <c r="I71" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>88</v>
       </c>
       <c r="B72" t="s">
         <v>89</v>
       </c>
-      <c r="F72" t="s">
-        <v>186</v>
-      </c>
-      <c r="G72" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>186</v>
+      </c>
+      <c r="I72" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>92</v>
       </c>
       <c r="B73" t="s">
         <v>92</v>
       </c>
-      <c r="F73" t="s">
-        <v>186</v>
-      </c>
-      <c r="G73" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>186</v>
+      </c>
+      <c r="I73" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>99</v>
       </c>
       <c r="B74" t="s">
         <v>93</v>
       </c>
-      <c r="F74" t="s">
-        <v>186</v>
-      </c>
-      <c r="G74" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" t="s">
+        <v>186</v>
+      </c>
+      <c r="I74" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>100</v>
       </c>
       <c r="B75" t="s">
         <v>101</v>
       </c>
-      <c r="F75" t="s">
-        <v>186</v>
-      </c>
-      <c r="G75" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>186</v>
+      </c>
+      <c r="I75" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>92</v>
       </c>
       <c r="B76" t="s">
         <v>94</v>
       </c>
-      <c r="F76" t="s">
-        <v>186</v>
-      </c>
-      <c r="G76" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
+        <v>186</v>
+      </c>
+      <c r="I76" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>104</v>
       </c>
       <c r="B77" t="s">
         <v>105</v>
       </c>
-      <c r="F77" t="s">
-        <v>186</v>
-      </c>
-      <c r="G77" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>186</v>
+      </c>
+      <c r="I77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>92</v>
       </c>
       <c r="B78" t="s">
         <v>108</v>
       </c>
-      <c r="F78" t="s">
-        <v>186</v>
-      </c>
-      <c r="G78" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>186</v>
+      </c>
+      <c r="I78" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>92</v>
       </c>
       <c r="B79" t="s">
         <v>95</v>
       </c>
-      <c r="F79" t="s">
-        <v>186</v>
-      </c>
-      <c r="G79" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79" t="s">
+        <v>186</v>
+      </c>
+      <c r="I79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>92</v>
       </c>
       <c r="B80" t="s">
         <v>102</v>
       </c>
-      <c r="F80" t="s">
-        <v>186</v>
-      </c>
-      <c r="G80" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>186</v>
+      </c>
+      <c r="I80" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>197</v>
       </c>
       <c r="B81" t="s">
         <v>198</v>
       </c>
-      <c r="F81" t="s">
-        <v>186</v>
-      </c>
-      <c r="G81" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>186</v>
+      </c>
+      <c r="I81" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>92</v>
       </c>
       <c r="B82" t="s">
         <v>103</v>
       </c>
-      <c r="F82" t="s">
-        <v>186</v>
-      </c>
-      <c r="G82" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>186</v>
+      </c>
+      <c r="I82" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>92</v>
       </c>
       <c r="B83" t="s">
         <v>96</v>
       </c>
-      <c r="F83" t="s">
-        <v>186</v>
-      </c>
-      <c r="G83" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>186</v>
+      </c>
+      <c r="I83" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>106</v>
       </c>
       <c r="B84" t="s">
         <v>107</v>
       </c>
-      <c r="F84" t="s">
-        <v>186</v>
-      </c>
-      <c r="G84" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" t="s">
+        <v>186</v>
+      </c>
+      <c r="I84" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>97</v>
       </c>
       <c r="B85" t="s">
         <v>98</v>
       </c>
-      <c r="F85" t="s">
-        <v>186</v>
-      </c>
-      <c r="G85" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>186</v>
+      </c>
+      <c r="I85" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>125</v>
       </c>
       <c r="B86" t="s">
         <v>125</v>
       </c>
-      <c r="F86" t="s">
-        <v>186</v>
-      </c>
-      <c r="G86" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>186</v>
+      </c>
+      <c r="I86" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>113</v>
       </c>
       <c r="B87" t="s">
         <v>114</v>
       </c>
-      <c r="F87" t="s">
-        <v>186</v>
-      </c>
-      <c r="G87" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
+        <v>186</v>
+      </c>
+      <c r="I87" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>113</v>
       </c>
       <c r="B88" t="s">
         <v>115</v>
       </c>
-      <c r="F88" t="s">
-        <v>186</v>
-      </c>
-      <c r="G88" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>186</v>
+      </c>
+      <c r="I88" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>113</v>
       </c>
       <c r="B89" t="s">
         <v>116</v>
       </c>
-      <c r="F89" t="s">
-        <v>186</v>
-      </c>
-      <c r="G89" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>186</v>
+      </c>
+      <c r="I89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>109</v>
       </c>
       <c r="B90" t="s">
         <v>110</v>
       </c>
-      <c r="F90" t="s">
-        <v>186</v>
-      </c>
-      <c r="G90" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90" t="s">
+        <v>186</v>
+      </c>
+      <c r="I90" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>117</v>
       </c>
       <c r="B91" t="s">
         <v>118</v>
       </c>
-      <c r="F91" t="s">
-        <v>186</v>
-      </c>
-      <c r="G91" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>186</v>
+      </c>
+      <c r="I91" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>119</v>
       </c>
       <c r="B92" t="s">
         <v>120</v>
       </c>
-      <c r="F92" t="s">
-        <v>186</v>
-      </c>
-      <c r="G92" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>186</v>
+      </c>
+      <c r="I92" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>111</v>
       </c>
       <c r="B93" t="s">
         <v>112</v>
       </c>
-      <c r="F93" t="s">
-        <v>186</v>
-      </c>
-      <c r="G93" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>186</v>
+      </c>
+      <c r="I93" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>121</v>
       </c>
       <c r="B94" t="s">
         <v>122</v>
       </c>
-      <c r="F94" t="s">
-        <v>186</v>
-      </c>
-      <c r="G94" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" t="s">
+        <v>186</v>
+      </c>
+      <c r="I94" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>126</v>
       </c>
       <c r="B95" t="s">
         <v>127</v>
       </c>
-      <c r="F95" t="s">
-        <v>186</v>
-      </c>
-      <c r="G95" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95" t="s">
+        <v>186</v>
+      </c>
+      <c r="I95" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>123</v>
       </c>
       <c r="B96" t="s">
         <v>124</v>
       </c>
-      <c r="F96" t="s">
-        <v>186</v>
-      </c>
-      <c r="G96" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96" t="s">
+        <v>186</v>
+      </c>
+      <c r="I96" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>125</v>
       </c>
       <c r="B97" t="s">
         <v>128</v>
       </c>
-      <c r="F97" t="s">
-        <v>186</v>
-      </c>
-      <c r="G97" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97" t="s">
+        <v>186</v>
+      </c>
+      <c r="I97" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>129</v>
       </c>
       <c r="B98" t="s">
         <v>128</v>
       </c>
-      <c r="F98" t="s">
-        <v>186</v>
-      </c>
-      <c r="G98" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" t="s">
+        <v>186</v>
+      </c>
+      <c r="I98" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>132</v>
       </c>
       <c r="B99" t="s">
         <v>133</v>
       </c>
-      <c r="F99" t="s">
-        <v>186</v>
-      </c>
-      <c r="G99" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99" t="s">
+        <v>186</v>
+      </c>
+      <c r="I99" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>132</v>
       </c>
       <c r="B100" t="s">
         <v>134</v>
       </c>
-      <c r="F100" t="s">
-        <v>186</v>
-      </c>
-      <c r="G100" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100" t="s">
+        <v>186</v>
+      </c>
+      <c r="I100" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>132</v>
       </c>
       <c r="B101" t="s">
         <v>135</v>
       </c>
-      <c r="F101" t="s">
-        <v>186</v>
-      </c>
-      <c r="G101" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101" t="s">
+        <v>186</v>
+      </c>
+      <c r="I101" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>132</v>
       </c>
       <c r="B102" t="s">
         <v>136</v>
       </c>
-      <c r="F102" t="s">
-        <v>186</v>
-      </c>
-      <c r="G102" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102" t="s">
+        <v>186</v>
+      </c>
+      <c r="I102" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>132</v>
       </c>
       <c r="B103" t="s">
         <v>137</v>
       </c>
-      <c r="F103" t="s">
-        <v>186</v>
-      </c>
-      <c r="G103" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H103" t="s">
+        <v>186</v>
+      </c>
+      <c r="I103" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>132</v>
       </c>
       <c r="B104" t="s">
         <v>138</v>
       </c>
-      <c r="F104" t="s">
-        <v>186</v>
-      </c>
-      <c r="G104" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104" t="s">
+        <v>186</v>
+      </c>
+      <c r="I104" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>130</v>
       </c>
       <c r="B105" t="s">
         <v>131</v>
       </c>
-      <c r="F105" t="s">
-        <v>186</v>
-      </c>
-      <c r="G105" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H105" t="s">
+        <v>186</v>
+      </c>
+      <c r="I105" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>144</v>
       </c>
       <c r="B106" t="s">
         <v>144</v>
       </c>
-      <c r="F106" t="s">
-        <v>186</v>
-      </c>
-      <c r="G106" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>186</v>
+      </c>
+      <c r="I106" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>139</v>
       </c>
       <c r="B107" t="s">
         <v>140</v>
       </c>
-      <c r="F107" t="s">
-        <v>186</v>
-      </c>
-      <c r="G107" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107" t="s">
+        <v>186</v>
+      </c>
+      <c r="I107" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>141</v>
       </c>
       <c r="B108" t="s">
         <v>142</v>
       </c>
-      <c r="F108" t="s">
-        <v>186</v>
-      </c>
-      <c r="G108" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108" t="s">
+        <v>186</v>
+      </c>
+      <c r="I108" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>143</v>
       </c>
       <c r="B109" t="s">
         <v>208</v>
       </c>
-      <c r="F109" t="s">
-        <v>186</v>
-      </c>
-      <c r="G109" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109" t="s">
+        <v>186</v>
+      </c>
+      <c r="I109" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>160</v>
       </c>
@@ -2599,131 +2631,130 @@
       <c r="E110" t="s">
         <v>186</v>
       </c>
-      <c r="F110" t="s">
-        <v>186</v>
-      </c>
       <c r="G110" t="s">
+        <v>186</v>
+      </c>
+      <c r="H110" t="s">
+        <v>186</v>
+      </c>
+      <c r="I110" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>160</v>
       </c>
       <c r="B111" t="s">
         <v>161</v>
       </c>
-      <c r="F111" t="s">
-        <v>186</v>
-      </c>
-      <c r="G111" t="s">
+      <c r="H111" t="s">
+        <v>186</v>
+      </c>
+      <c r="I111" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>145</v>
       </c>
       <c r="B112" t="s">
         <v>146</v>
       </c>
-      <c r="F112" t="s">
-        <v>186</v>
-      </c>
-      <c r="G112" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H112" t="s">
+        <v>186</v>
+      </c>
+      <c r="I112" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>147</v>
       </c>
       <c r="B113" t="s">
         <v>148</v>
       </c>
-      <c r="F113" t="s">
-        <v>186</v>
-      </c>
-      <c r="G113" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H113" t="s">
+        <v>186</v>
+      </c>
+      <c r="I113" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>192</v>
       </c>
       <c r="B114" t="s">
         <v>193</v>
       </c>
-      <c r="F114" t="s">
-        <v>186</v>
-      </c>
-      <c r="G114" t="s">
+      <c r="H114" t="s">
+        <v>186</v>
+      </c>
+      <c r="I114" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>149</v>
       </c>
       <c r="B115" t="s">
         <v>150</v>
       </c>
-      <c r="F115" t="s">
-        <v>186</v>
-      </c>
-      <c r="G115" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H115" t="s">
+        <v>186</v>
+      </c>
+      <c r="I115" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>151</v>
       </c>
       <c r="B116" t="s">
         <v>209</v>
       </c>
-      <c r="F116" t="s">
-        <v>186</v>
-      </c>
-      <c r="G116" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H116" t="s">
+        <v>186</v>
+      </c>
+      <c r="I116" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>168</v>
       </c>
       <c r="B117" t="s">
         <v>167</v>
       </c>
-      <c r="F117" t="s">
-        <v>186</v>
-      </c>
-      <c r="G117" t="s">
+      <c r="H117" t="s">
+        <v>186</v>
+      </c>
+      <c r="I117" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>152</v>
       </c>
       <c r="B118" t="s">
         <v>153</v>
       </c>
-      <c r="F118" t="s">
-        <v>186</v>
-      </c>
-      <c r="G118" t="s">
+      <c r="H118" t="s">
+        <v>186</v>
+      </c>
+      <c r="I118" t="s">
         <v>157</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G118">
-    <sortState ref="A2:G118">
-      <sortCondition ref="B1:B118"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:I118"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added BasicPlus gapp (geotagger + Basic), updated docs to match, Added SplitCategory field to merged.txt
</commit_message>
<xml_diff>
--- a/LanguageResources/docs/OpenSextant Entities.xlsx
+++ b/LanguageResources/docs/OpenSextant Entities.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Hierarchy Roots" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$I$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$J$118</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="219">
   <si>
     <t>Crime</t>
   </si>
@@ -672,6 +672,9 @@
   </si>
   <si>
     <t>Basic</t>
+  </si>
+  <si>
+    <t>BasicPlus</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,13 +1026,14 @@
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>154</v>
       </c>
@@ -1046,369 +1050,372 @@
         <v>217</v>
       </c>
       <c r="F1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G1" t="s">
         <v>163</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>200</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>201</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
-        <v>186</v>
-      </c>
       <c r="I2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
-        <v>186</v>
-      </c>
       <c r="I3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
-        <v>186</v>
-      </c>
       <c r="I4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" t="s">
-        <v>186</v>
-      </c>
       <c r="I5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" t="s">
-        <v>186</v>
-      </c>
       <c r="I6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" t="s">
-        <v>186</v>
-      </c>
       <c r="I7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" t="s">
-        <v>186</v>
-      </c>
       <c r="I8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="H9" t="s">
-        <v>186</v>
-      </c>
       <c r="I9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="H10" t="s">
-        <v>186</v>
-      </c>
       <c r="I10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="H11" t="s">
-        <v>186</v>
-      </c>
       <c r="I11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="H12" t="s">
-        <v>186</v>
-      </c>
       <c r="I12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>214</v>
       </c>
       <c r="B13" t="s">
         <v>215</v>
       </c>
-      <c r="H13" t="s">
-        <v>186</v>
-      </c>
       <c r="I13" t="s">
+        <v>186</v>
+      </c>
+      <c r="J13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>212</v>
       </c>
       <c r="B14" t="s">
         <v>213</v>
       </c>
-      <c r="H14" t="s">
-        <v>186</v>
-      </c>
       <c r="I14" t="s">
+        <v>186</v>
+      </c>
+      <c r="J14" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>210</v>
       </c>
       <c r="B15" t="s">
         <v>211</v>
       </c>
-      <c r="H15" t="s">
-        <v>186</v>
-      </c>
       <c r="I15" t="s">
+        <v>186</v>
+      </c>
+      <c r="J15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="H16" t="s">
-        <v>186</v>
-      </c>
       <c r="I16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="H17" t="s">
-        <v>186</v>
-      </c>
       <c r="I17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="H18" t="s">
-        <v>186</v>
-      </c>
       <c r="I18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="H19" t="s">
-        <v>186</v>
-      </c>
       <c r="I19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="H20" t="s">
-        <v>186</v>
-      </c>
       <c r="I20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="H21" t="s">
-        <v>186</v>
-      </c>
       <c r="I21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="H22" t="s">
-        <v>186</v>
-      </c>
       <c r="I22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="H23" t="s">
-        <v>186</v>
-      </c>
       <c r="I23" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="H24" t="s">
-        <v>186</v>
-      </c>
       <c r="I24" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
-      <c r="H25" t="s">
-        <v>186</v>
-      </c>
       <c r="I25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="H26" t="s">
-        <v>186</v>
-      </c>
       <c r="I26" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>159</v>
       </c>
@@ -1434,10 +1441,13 @@
         <v>186</v>
       </c>
       <c r="I27" t="s">
+        <v>186</v>
+      </c>
+      <c r="J27" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>199</v>
       </c>
@@ -1457,108 +1467,111 @@
         <v>186</v>
       </c>
       <c r="I28" t="s">
+        <v>186</v>
+      </c>
+      <c r="J28" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="H29" t="s">
-        <v>186</v>
-      </c>
       <c r="I29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
       <c r="B30" t="s">
         <v>43</v>
       </c>
-      <c r="H30" t="s">
-        <v>186</v>
-      </c>
       <c r="I30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
       <c r="B31" t="s">
         <v>38</v>
       </c>
-      <c r="H31" t="s">
-        <v>186</v>
-      </c>
       <c r="I31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
       </c>
-      <c r="H32" t="s">
-        <v>186</v>
-      </c>
       <c r="I32" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>41</v>
       </c>
-      <c r="H33" t="s">
-        <v>186</v>
-      </c>
       <c r="I33" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
       <c r="B34" t="s">
         <v>44</v>
       </c>
-      <c r="H34" t="s">
-        <v>186</v>
-      </c>
       <c r="I34" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>165</v>
       </c>
       <c r="B35" t="s">
         <v>164</v>
       </c>
-      <c r="H35" t="s">
-        <v>186</v>
-      </c>
       <c r="I35" t="s">
+        <v>186</v>
+      </c>
+      <c r="J35" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>189</v>
       </c>
@@ -1568,17 +1581,20 @@
       <c r="E36" t="s">
         <v>186</v>
       </c>
-      <c r="G36" t="s">
+      <c r="F36" t="s">
         <v>186</v>
       </c>
       <c r="H36" t="s">
         <v>186</v>
       </c>
       <c r="I36" t="s">
+        <v>186</v>
+      </c>
+      <c r="J36" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>184</v>
       </c>
@@ -1588,17 +1604,20 @@
       <c r="E37" t="s">
         <v>186</v>
       </c>
-      <c r="G37" t="s">
+      <c r="F37" t="s">
         <v>186</v>
       </c>
       <c r="H37" t="s">
         <v>186</v>
       </c>
       <c r="I37" t="s">
+        <v>186</v>
+      </c>
+      <c r="J37" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -1608,241 +1627,244 @@
       <c r="E38" t="s">
         <v>186</v>
       </c>
-      <c r="G38" t="s">
+      <c r="F38" t="s">
         <v>186</v>
       </c>
       <c r="H38" t="s">
         <v>186</v>
       </c>
       <c r="I38" t="s">
+        <v>186</v>
+      </c>
+      <c r="J38" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
       <c r="B39" t="s">
         <v>46</v>
       </c>
-      <c r="H39" t="s">
-        <v>186</v>
-      </c>
       <c r="I39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
       </c>
-      <c r="H40" t="s">
-        <v>186</v>
-      </c>
       <c r="I40" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>170</v>
       </c>
       <c r="B41" t="s">
         <v>169</v>
       </c>
-      <c r="H41" t="s">
-        <v>186</v>
-      </c>
       <c r="I41" t="s">
+        <v>186</v>
+      </c>
+      <c r="J41" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>176</v>
       </c>
       <c r="B42" t="s">
         <v>175</v>
       </c>
-      <c r="H42" t="s">
-        <v>186</v>
-      </c>
       <c r="I42" t="s">
+        <v>186</v>
+      </c>
+      <c r="J42" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>172</v>
       </c>
       <c r="B43" t="s">
         <v>171</v>
       </c>
-      <c r="H43" t="s">
-        <v>186</v>
-      </c>
       <c r="I43" t="s">
+        <v>186</v>
+      </c>
+      <c r="J43" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>174</v>
       </c>
       <c r="B44" t="s">
         <v>173</v>
       </c>
-      <c r="H44" t="s">
-        <v>186</v>
-      </c>
       <c r="I44" t="s">
+        <v>186</v>
+      </c>
+      <c r="J44" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>73</v>
       </c>
       <c r="B45" t="s">
         <v>73</v>
       </c>
-      <c r="H45" t="s">
-        <v>186</v>
-      </c>
       <c r="I45" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
       <c r="B46" t="s">
         <v>54</v>
       </c>
-      <c r="H46" t="s">
-        <v>186</v>
-      </c>
       <c r="I46" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>57</v>
       </c>
       <c r="B47" t="s">
         <v>58</v>
       </c>
-      <c r="H47" t="s">
-        <v>186</v>
-      </c>
       <c r="I47" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>61</v>
       </c>
       <c r="B48" t="s">
         <v>62</v>
       </c>
-      <c r="H48" t="s">
-        <v>186</v>
-      </c>
       <c r="I48" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
       <c r="B49" t="s">
         <v>64</v>
       </c>
-      <c r="H49" t="s">
-        <v>186</v>
-      </c>
       <c r="I49" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>65</v>
       </c>
       <c r="B50" t="s">
         <v>66</v>
       </c>
-      <c r="H50" t="s">
-        <v>186</v>
-      </c>
       <c r="I50" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J50" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>67</v>
       </c>
       <c r="B51" t="s">
         <v>68</v>
       </c>
-      <c r="H51" t="s">
-        <v>186</v>
-      </c>
       <c r="I51" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J51" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
       </c>
-      <c r="H52" t="s">
-        <v>186</v>
-      </c>
       <c r="I52" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>80</v>
       </c>
       <c r="B53" t="s">
         <v>81</v>
       </c>
-      <c r="H53" t="s">
-        <v>186</v>
-      </c>
       <c r="I53" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J53" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>195</v>
       </c>
       <c r="B54" t="s">
         <v>196</v>
       </c>
-      <c r="H54" t="s">
-        <v>186</v>
-      </c>
       <c r="I54" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -1852,773 +1874,776 @@
       <c r="E55" t="s">
         <v>186</v>
       </c>
-      <c r="G55" t="s">
+      <c r="F55" t="s">
         <v>186</v>
       </c>
       <c r="H55" t="s">
         <v>186</v>
       </c>
       <c r="I55" t="s">
+        <v>186</v>
+      </c>
+      <c r="J55" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>74</v>
       </c>
       <c r="B56" t="s">
         <v>75</v>
       </c>
-      <c r="H56" t="s">
-        <v>186</v>
-      </c>
       <c r="I56" t="s">
+        <v>186</v>
+      </c>
+      <c r="J56" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>69</v>
       </c>
       <c r="B57" t="s">
         <v>70</v>
       </c>
-      <c r="H57" t="s">
-        <v>186</v>
-      </c>
       <c r="I57" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>82</v>
       </c>
       <c r="B58" t="s">
         <v>83</v>
       </c>
-      <c r="H58" t="s">
-        <v>186</v>
-      </c>
       <c r="I58" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J58" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>49</v>
       </c>
       <c r="B59" t="s">
         <v>50</v>
       </c>
-      <c r="H59" t="s">
-        <v>186</v>
-      </c>
       <c r="I59" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J59" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>49</v>
       </c>
       <c r="B60" t="s">
         <v>51</v>
       </c>
-      <c r="H60" t="s">
-        <v>186</v>
-      </c>
       <c r="I60" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J60" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>49</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
       </c>
-      <c r="H61" t="s">
-        <v>186</v>
-      </c>
       <c r="I61" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J61" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>71</v>
       </c>
       <c r="B62" t="s">
         <v>72</v>
       </c>
-      <c r="H62" t="s">
-        <v>186</v>
-      </c>
       <c r="I62" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>203</v>
       </c>
       <c r="B63" t="s">
         <v>204</v>
       </c>
-      <c r="H63" t="s">
-        <v>186</v>
-      </c>
       <c r="I63" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J63" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
       </c>
       <c r="B64" t="s">
         <v>56</v>
       </c>
-      <c r="H64" t="s">
-        <v>186</v>
-      </c>
       <c r="I64" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J64" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
       <c r="B65" t="s">
         <v>205</v>
       </c>
-      <c r="H65" t="s">
-        <v>186</v>
-      </c>
       <c r="I65" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J65" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>76</v>
       </c>
       <c r="B66" t="s">
         <v>77</v>
       </c>
-      <c r="H66" t="s">
-        <v>186</v>
-      </c>
       <c r="I66" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>206</v>
       </c>
       <c r="B67" t="s">
         <v>207</v>
       </c>
-      <c r="H67" t="s">
-        <v>186</v>
-      </c>
       <c r="I67" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J67" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>78</v>
       </c>
       <c r="B68" t="s">
         <v>79</v>
       </c>
-      <c r="H68" t="s">
-        <v>186</v>
-      </c>
       <c r="I68" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J68" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>90</v>
       </c>
       <c r="B69" t="s">
         <v>91</v>
       </c>
-      <c r="H69" t="s">
-        <v>186</v>
-      </c>
       <c r="I69" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J69" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>84</v>
       </c>
       <c r="B70" t="s">
         <v>85</v>
       </c>
-      <c r="H70" t="s">
-        <v>186</v>
-      </c>
       <c r="I70" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>86</v>
       </c>
       <c r="B71" t="s">
         <v>87</v>
       </c>
-      <c r="H71" t="s">
-        <v>186</v>
-      </c>
       <c r="I71" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J71" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>88</v>
       </c>
       <c r="B72" t="s">
         <v>89</v>
       </c>
-      <c r="H72" t="s">
-        <v>186</v>
-      </c>
       <c r="I72" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J72" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>92</v>
       </c>
       <c r="B73" t="s">
         <v>92</v>
       </c>
-      <c r="H73" t="s">
-        <v>186</v>
-      </c>
       <c r="I73" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J73" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>99</v>
       </c>
       <c r="B74" t="s">
         <v>93</v>
       </c>
-      <c r="H74" t="s">
-        <v>186</v>
-      </c>
       <c r="I74" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J74" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>100</v>
       </c>
       <c r="B75" t="s">
         <v>101</v>
       </c>
-      <c r="H75" t="s">
-        <v>186</v>
-      </c>
       <c r="I75" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J75" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>92</v>
       </c>
       <c r="B76" t="s">
         <v>94</v>
       </c>
-      <c r="H76" t="s">
-        <v>186</v>
-      </c>
       <c r="I76" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J76" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>104</v>
       </c>
       <c r="B77" t="s">
         <v>105</v>
       </c>
-      <c r="H77" t="s">
-        <v>186</v>
-      </c>
       <c r="I77" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>92</v>
       </c>
       <c r="B78" t="s">
         <v>108</v>
       </c>
-      <c r="H78" t="s">
-        <v>186</v>
-      </c>
       <c r="I78" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J78" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>92</v>
       </c>
       <c r="B79" t="s">
         <v>95</v>
       </c>
-      <c r="H79" t="s">
-        <v>186</v>
-      </c>
       <c r="I79" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>92</v>
       </c>
       <c r="B80" t="s">
         <v>102</v>
       </c>
-      <c r="H80" t="s">
-        <v>186</v>
-      </c>
       <c r="I80" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J80" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>197</v>
       </c>
       <c r="B81" t="s">
         <v>198</v>
       </c>
-      <c r="H81" t="s">
-        <v>186</v>
-      </c>
       <c r="I81" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J81" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>92</v>
       </c>
       <c r="B82" t="s">
         <v>103</v>
       </c>
-      <c r="H82" t="s">
-        <v>186</v>
-      </c>
       <c r="I82" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J82" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>92</v>
       </c>
       <c r="B83" t="s">
         <v>96</v>
       </c>
-      <c r="H83" t="s">
-        <v>186</v>
-      </c>
       <c r="I83" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J83" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>106</v>
       </c>
       <c r="B84" t="s">
         <v>107</v>
       </c>
-      <c r="H84" t="s">
-        <v>186</v>
-      </c>
       <c r="I84" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J84" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>97</v>
       </c>
       <c r="B85" t="s">
         <v>98</v>
       </c>
-      <c r="H85" t="s">
-        <v>186</v>
-      </c>
       <c r="I85" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J85" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>125</v>
       </c>
       <c r="B86" t="s">
         <v>125</v>
       </c>
-      <c r="H86" t="s">
-        <v>186</v>
-      </c>
       <c r="I86" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J86" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>113</v>
       </c>
       <c r="B87" t="s">
         <v>114</v>
       </c>
-      <c r="H87" t="s">
-        <v>186</v>
-      </c>
       <c r="I87" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J87" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>113</v>
       </c>
       <c r="B88" t="s">
         <v>115</v>
       </c>
-      <c r="H88" t="s">
-        <v>186</v>
-      </c>
       <c r="I88" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J88" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>113</v>
       </c>
       <c r="B89" t="s">
         <v>116</v>
       </c>
-      <c r="H89" t="s">
-        <v>186</v>
-      </c>
       <c r="I89" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>109</v>
       </c>
       <c r="B90" t="s">
         <v>110</v>
       </c>
-      <c r="H90" t="s">
-        <v>186</v>
-      </c>
       <c r="I90" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J90" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>117</v>
       </c>
       <c r="B91" t="s">
         <v>118</v>
       </c>
-      <c r="H91" t="s">
-        <v>186</v>
-      </c>
       <c r="I91" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J91" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>119</v>
       </c>
       <c r="B92" t="s">
         <v>120</v>
       </c>
-      <c r="H92" t="s">
-        <v>186</v>
-      </c>
       <c r="I92" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J92" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>111</v>
       </c>
       <c r="B93" t="s">
         <v>112</v>
       </c>
-      <c r="H93" t="s">
-        <v>186</v>
-      </c>
       <c r="I93" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J93" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>121</v>
       </c>
       <c r="B94" t="s">
         <v>122</v>
       </c>
-      <c r="H94" t="s">
-        <v>186</v>
-      </c>
       <c r="I94" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J94" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>126</v>
       </c>
       <c r="B95" t="s">
         <v>127</v>
       </c>
-      <c r="H95" t="s">
-        <v>186</v>
-      </c>
       <c r="I95" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J95" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>123</v>
       </c>
       <c r="B96" t="s">
         <v>124</v>
       </c>
-      <c r="H96" t="s">
-        <v>186</v>
-      </c>
       <c r="I96" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J96" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>125</v>
       </c>
       <c r="B97" t="s">
         <v>128</v>
       </c>
-      <c r="H97" t="s">
-        <v>186</v>
-      </c>
       <c r="I97" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J97" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>129</v>
       </c>
       <c r="B98" t="s">
         <v>128</v>
       </c>
-      <c r="H98" t="s">
-        <v>186</v>
-      </c>
       <c r="I98" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J98" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>132</v>
       </c>
       <c r="B99" t="s">
         <v>133</v>
       </c>
-      <c r="H99" t="s">
-        <v>186</v>
-      </c>
       <c r="I99" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J99" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>132</v>
       </c>
       <c r="B100" t="s">
         <v>134</v>
       </c>
-      <c r="H100" t="s">
-        <v>186</v>
-      </c>
       <c r="I100" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J100" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>132</v>
       </c>
       <c r="B101" t="s">
         <v>135</v>
       </c>
-      <c r="H101" t="s">
-        <v>186</v>
-      </c>
       <c r="I101" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J101" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>132</v>
       </c>
       <c r="B102" t="s">
         <v>136</v>
       </c>
-      <c r="H102" t="s">
-        <v>186</v>
-      </c>
       <c r="I102" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J102" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>132</v>
       </c>
       <c r="B103" t="s">
         <v>137</v>
       </c>
-      <c r="H103" t="s">
-        <v>186</v>
-      </c>
       <c r="I103" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J103" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>132</v>
       </c>
       <c r="B104" t="s">
         <v>138</v>
       </c>
-      <c r="H104" t="s">
-        <v>186</v>
-      </c>
       <c r="I104" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J104" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>130</v>
       </c>
       <c r="B105" t="s">
         <v>131</v>
       </c>
-      <c r="H105" t="s">
-        <v>186</v>
-      </c>
       <c r="I105" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J105" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>144</v>
       </c>
       <c r="B106" t="s">
         <v>144</v>
       </c>
-      <c r="H106" t="s">
-        <v>186</v>
-      </c>
       <c r="I106" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J106" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>139</v>
       </c>
       <c r="B107" t="s">
         <v>140</v>
       </c>
-      <c r="H107" t="s">
-        <v>186</v>
-      </c>
       <c r="I107" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J107" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>141</v>
       </c>
       <c r="B108" t="s">
         <v>142</v>
       </c>
-      <c r="H108" t="s">
-        <v>186</v>
-      </c>
       <c r="I108" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J108" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>143</v>
       </c>
       <c r="B109" t="s">
         <v>208</v>
       </c>
-      <c r="H109" t="s">
-        <v>186</v>
-      </c>
       <c r="I109" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J109" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>160</v>
       </c>
@@ -2631,130 +2656,133 @@
       <c r="E110" t="s">
         <v>186</v>
       </c>
-      <c r="G110" t="s">
+      <c r="F110" t="s">
         <v>186</v>
       </c>
       <c r="H110" t="s">
         <v>186</v>
       </c>
       <c r="I110" t="s">
+        <v>186</v>
+      </c>
+      <c r="J110" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>160</v>
       </c>
       <c r="B111" t="s">
         <v>161</v>
       </c>
-      <c r="H111" t="s">
-        <v>186</v>
-      </c>
       <c r="I111" t="s">
+        <v>186</v>
+      </c>
+      <c r="J111" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>145</v>
       </c>
       <c r="B112" t="s">
         <v>146</v>
       </c>
-      <c r="H112" t="s">
-        <v>186</v>
-      </c>
       <c r="I112" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J112" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>147</v>
       </c>
       <c r="B113" t="s">
         <v>148</v>
       </c>
-      <c r="H113" t="s">
-        <v>186</v>
-      </c>
       <c r="I113" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J113" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>192</v>
       </c>
       <c r="B114" t="s">
         <v>193</v>
       </c>
-      <c r="H114" t="s">
-        <v>186</v>
-      </c>
       <c r="I114" t="s">
+        <v>186</v>
+      </c>
+      <c r="J114" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>149</v>
       </c>
       <c r="B115" t="s">
         <v>150</v>
       </c>
-      <c r="H115" t="s">
-        <v>186</v>
-      </c>
       <c r="I115" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J115" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>151</v>
       </c>
       <c r="B116" t="s">
         <v>209</v>
       </c>
-      <c r="H116" t="s">
-        <v>186</v>
-      </c>
       <c r="I116" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="J116" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>168</v>
       </c>
       <c r="B117" t="s">
         <v>167</v>
       </c>
-      <c r="H117" t="s">
-        <v>186</v>
-      </c>
       <c r="I117" t="s">
+        <v>186</v>
+      </c>
+      <c r="J117" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>152</v>
       </c>
       <c r="B118" t="s">
         <v>153</v>
       </c>
-      <c r="H118" t="s">
-        <v>186</v>
-      </c>
       <c r="I118" t="s">
+        <v>186</v>
+      </c>
+      <c r="J118" t="s">
         <v>157</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I118"/>
+  <autoFilter ref="A1:J118"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>